<commit_message>
Add 5 user stories
</commit_message>
<xml_diff>
--- a/historias-de-usuario.xlsx
+++ b/historias-de-usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enzocazenave/Desktop/repos/dolar-historico/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A2B01E-1823-4640-AF6B-D81F3F5242F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD84DBF-0137-3943-BA66-D53689298C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{61342663-3276-C043-B24B-34E2E0177A3C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="35">
   <si>
     <t>COMO</t>
   </si>
@@ -108,6 +108,39 @@
   </si>
   <si>
     <t>establecer prioridades</t>
+  </si>
+  <si>
+    <t>desarrollador</t>
+  </si>
+  <si>
+    <t>desarrollar un sitio web</t>
+  </si>
+  <si>
+    <t>redireccionar a apple store o play store y explicar en que consiste la app</t>
+  </si>
+  <si>
+    <t>tener la posibilidad de compartir una cotizacion de una moneda</t>
+  </si>
+  <si>
+    <t>informar a amigos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tener la posilibilidad de visualizar en un grafico la variacion de cotizacion de una moneda </t>
+  </si>
+  <si>
+    <t>tener información más gráfica</t>
+  </si>
+  <si>
+    <t>tener un conversor</t>
+  </si>
+  <si>
+    <t>convertir rapida e intuitivamente un monto en pesos a la divisa que elija</t>
+  </si>
+  <si>
+    <t>que la aplicacion funcione iOS y android</t>
+  </si>
+  <si>
+    <t>tener un mayor alcance de personas</t>
   </si>
 </sst>
 </file>
@@ -273,7 +306,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9756EE13-56C9-AA48-A1D5-BADF13C0143C}">
   <dimension ref="B2:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="32" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1311,7 +1344,9 @@
       <c r="B53" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C53" s="4"/>
+      <c r="C53" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E53" s="1" t="s">
         <v>0</v>
       </c>
@@ -1325,7 +1360,9 @@
       <c r="B54" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C54" s="4"/>
+      <c r="C54" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E54" s="1" t="s">
         <v>1</v>
       </c>
@@ -1339,7 +1376,9 @@
       <c r="B55" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C55" s="4"/>
+      <c r="C55" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="E55" s="1" t="s">
         <v>2</v>
       </c>
@@ -1373,7 +1412,9 @@
       <c r="B58" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="8"/>
+      <c r="C58" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E58" s="1" t="s">
         <v>0</v>
       </c>
@@ -1387,7 +1428,9 @@
       <c r="B59" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="8"/>
+      <c r="C59" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="E59" s="1" t="s">
         <v>1</v>
       </c>
@@ -1401,7 +1444,9 @@
       <c r="B60" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="8"/>
+      <c r="C60" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="E60" s="1" t="s">
         <v>2</v>
       </c>
@@ -1435,7 +1480,9 @@
       <c r="B63" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C63" s="8"/>
+      <c r="C63" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E63" s="1" t="s">
         <v>0</v>
       </c>
@@ -1449,7 +1496,9 @@
       <c r="B64" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C64" s="8"/>
+      <c r="C64" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="E64" s="1" t="s">
         <v>1</v>
       </c>
@@ -1463,7 +1512,9 @@
       <c r="B65" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="8"/>
+      <c r="C65" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="E65" s="1" t="s">
         <v>2</v>
       </c>
@@ -1497,7 +1548,9 @@
       <c r="B68" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C68" s="8"/>
+      <c r="C68" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E68" s="1" t="s">
         <v>0</v>
       </c>
@@ -1511,7 +1564,9 @@
       <c r="B69" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C69" s="8"/>
+      <c r="C69" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="E69" s="1" t="s">
         <v>1</v>
       </c>
@@ -1525,7 +1580,9 @@
       <c r="B70" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C70" s="8"/>
+      <c r="C70" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="E70" s="1" t="s">
         <v>2</v>
       </c>
@@ -1559,7 +1616,9 @@
       <c r="B73" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C73" s="8"/>
+      <c r="C73" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="E73" s="1" t="s">
         <v>0</v>
       </c>
@@ -1573,7 +1632,9 @@
       <c r="B74" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="8"/>
+      <c r="C74" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="E74" s="1" t="s">
         <v>1</v>
       </c>
@@ -1587,7 +1648,9 @@
       <c r="B75" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C75" s="8"/>
+      <c r="C75" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="E75" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>